<commit_message>
Casi acabado el schema
</commit_message>
<xml_diff>
--- a/castilla_leon_1.xlsx
+++ b/castilla_leon_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="337">
   <si>
     <t xml:space="preserve">Pastelería Dolce Vita</t>
   </si>
@@ -1362,8 +1362,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2091,7 +2091,9 @@
       <c r="D19" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>186</v>
       </c>
@@ -2130,7 +2132,9 @@
       <c r="D20" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>195</v>
       </c>
@@ -2366,7 +2370,9 @@
       <c r="D26" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F26" s="1" t="s">
         <v>249</v>
       </c>

</xml_diff>